<commit_message>
Add login verification and globalExceptionHandler
</commit_message>
<xml_diff>
--- a/webbora-daily-report-service/src/test/resources/test.xlsx
+++ b/webbora-daily-report-service/src/test/resources/test.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jupiter/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jupiter/14.idea-workspace/daily-report/webbora-daily-report-service/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10D3A835-3621-5B4E-BD17-C70F39199CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE7CEB2-3095-B944-A009-4CECC125786E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="1920" windowWidth="19200" windowHeight="11820" xr2:uid="{67E005E8-4206-D740-836F-9912DC80484B}"/>
+    <workbookView xWindow="11300" yWindow="8400" windowWidth="15480" windowHeight="9820" activeTab="1" xr2:uid="{67E005E8-4206-D740-836F-9912DC80484B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="report1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -48,6 +49,36 @@
   </si>
   <si>
     <t>Jupiter</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>你好呀</t>
+  </si>
+  <si>
+    <t>hello world</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -71,7 +102,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -79,12 +110,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C153613C-8B91-F047-AD95-6B6AA499F6B9}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,4 +499,139 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14A806DD-AFA2-B64D-9A9C-9AA27F2EDEEA}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(excel): support .xlsb file format and update context paths
</commit_message>
<xml_diff>
--- a/webbora-daily-report-service/src/test/resources/test.xlsx
+++ b/webbora-daily-report-service/src/test/resources/test.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jupiter/14.idea-workspace/daily-report/webbora-daily-report-service/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE7CEB2-3095-B944-A009-4CECC125786E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3A3824-F5B9-B940-B650-4A3068A4344B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11300" yWindow="8400" windowWidth="15480" windowHeight="9820" activeTab="1" xr2:uid="{67E005E8-4206-D740-836F-9912DC80484B}"/>
+    <workbookView xWindow="5680" yWindow="4880" windowWidth="15480" windowHeight="9820" xr2:uid="{67E005E8-4206-D740-836F-9912DC80484B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="exhibit1" sheetId="1" r:id="rId1"/>
     <sheet name="report1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -37,19 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>Jupiter</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>a</t>
   </si>
@@ -79,14 +67,85 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Latest Close</t>
+  </si>
+  <si>
+    <t>Daily Pt Chg</t>
+  </si>
+  <si>
+    <t>Daily % Chg</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>DJIA</t>
+  </si>
+  <si>
+    <t>S&amp;P500</t>
+  </si>
+  <si>
+    <t>Nasdaq</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>UK FTSE</t>
+  </si>
+  <si>
+    <t>FR CAC</t>
+  </si>
+  <si>
+    <t>DE DAX</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>HSI</t>
+  </si>
+  <si>
+    <t>HSCEI</t>
+  </si>
+  <si>
+    <t>HSTECH</t>
+  </si>
+  <si>
+    <t>SH Composite</t>
+  </si>
+  <si>
+    <t>CSI300</t>
+  </si>
+  <si>
+    <t>Nikkei 225</t>
+  </si>
+  <si>
+    <t>TWII</t>
+  </si>
+  <si>
+    <t>KOSPI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -129,9 +188,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,37 +531,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C153613C-8B91-F047-AD95-6B6AA499F6B9}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="B2:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3">
+        <v>42225.32</v>
+      </c>
+      <c r="D4">
+        <v>235.4</v>
+      </c>
+      <c r="E4" s="4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5670.97</v>
+      </c>
+      <c r="D5">
+        <v>37.9</v>
+      </c>
+      <c r="E5" s="4">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3">
+        <v>17601.05</v>
+      </c>
+      <c r="D6">
+        <v>151.19999999999999</v>
+      </c>
+      <c r="E6" s="4">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3">
+        <v>8608.48</v>
+      </c>
+      <c r="D8">
+        <v>-26.3</v>
+      </c>
+      <c r="E8" s="4">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3">
+        <v>7858.83</v>
+      </c>
+      <c r="D9">
+        <v>-17.5</v>
+      </c>
+      <c r="E9" s="4">
+        <v>-2E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3">
+        <v>22390.84</v>
+      </c>
+      <c r="D10">
+        <v>-149.1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3">
+        <v>23202.53</v>
+      </c>
+      <c r="D12">
+        <v>-4.3</v>
+      </c>
+      <c r="E12" s="4">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>18</v>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3">
+        <v>8531.51</v>
+      </c>
+      <c r="D13">
+        <v>-5.8</v>
+      </c>
+      <c r="E13" s="4">
+        <v>-1E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="3">
+        <v>5426.44</v>
+      </c>
+      <c r="D14">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E14" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3350.13</v>
+      </c>
+      <c r="D15">
+        <v>1.7</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3">
+        <v>3884.39</v>
+      </c>
+      <c r="D16">
+        <v>-3.3</v>
+      </c>
+      <c r="E16" s="4">
+        <v>-1E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3">
+        <v>35725.870000000003</v>
+      </c>
+      <c r="D17">
+        <v>101.4</v>
+      </c>
+      <c r="E17" s="4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="3">
+        <v>21298.22</v>
+      </c>
+      <c r="D18">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2505.86</v>
+      </c>
+      <c r="D19">
+        <v>15.5</v>
+      </c>
+      <c r="E19" s="4">
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B11:E11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -505,7 +793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14A806DD-AFA2-B64D-9A9C-9AA27F2EDEEA}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -513,22 +801,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -539,16 +827,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>